<commit_message>
Modified Task 13 with workbook activities
</commit_message>
<xml_diff>
--- a/SourceCode/2023/August2023/Deekshitha/Task 13/Example.xlsx
+++ b/SourceCode/2023/August2023/Deekshitha/Task 13/Example.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA Course\RPA-Developer-in-30-Days\RPA-Developer-in-30-Days\SourceCode\2023\August2023\Deekshitha\Task 13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898C9862-0A0B-4AFD-AFF8-8C1A5F58E7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DF467B45-5D14-4EC5-8C78-62E0323D9435}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFA5D61-7B87-4190-B3A4-E05DFCEE6FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <x:bookViews>
+    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="0" activeTab="1" xr2:uid="{DF467B45-5D14-4EC5-8C78-62E0323D9435}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    </x:ext>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -31,82 +32,127 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <x:si>
+    <x:t>Month</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Food </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Monday</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ram</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Carrot</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Feb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tuesday</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nick</x:t>
+  </x:si>
+  <x:si>
+    <x:t>chiilies</x:t>
+  </x:si>
+  <x:si>
+    <x:t>March</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wednesday</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ghost</x:t>
+  </x:si>
+  <x:si>
+    <x:t>potato</x:t>
+  </x:si>
+  <x:si>
+    <x:t>April</x:t>
+  </x:si>
+  <x:si>
+    <x:t>May</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </x:cellStyleXfs>
+  <x:cellXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,89 +451,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541E7438-6C2A-41EB-A2A9-4DA7E13B1F35}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{541E7438-6C2A-41EB-A2A9-4DA7E13B1F35}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C6"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="D4" sqref="D4 D1:D4"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <x:c r="A3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <x:c r="A5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <x:c r="A6" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30140185-341A-4E5F-BD52-B3E84A479D5A}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{30140185-341A-4E5F-BD52-B3E84A479D5A}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:D6"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="E12" sqref="E12"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A6" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>